<commit_message>
work correct without der
</commit_message>
<xml_diff>
--- a/AP_DC_X-talk/dt_spectrum_results.xlsx
+++ b/AP_DC_X-talk/dt_spectrum_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hamamatsu S10362-11-100C apf" sheetId="1" r:id="rId1"/>
@@ -4250,8 +4250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM5522"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11624,8 +11624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12609,6 +12609,12 @@
       <c r="O43">
         <v>0.7</v>
       </c>
+      <c r="T43">
+        <v>0.3</v>
+      </c>
+      <c r="U43">
+        <v>0.7</v>
+      </c>
       <c r="X43">
         <v>1000</v>
       </c>

</xml_diff>

<commit_message>
add ER vs V - good model
</commit_message>
<xml_diff>
--- a/AP_DC_X-talk/dt_spectrum_results.xlsx
+++ b/AP_DC_X-talk/dt_spectrum_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hamamatsu S10362-11-100C apf" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="th" sheetId="3" r:id="rId3"/>
     <sheet name="Лист1" sheetId="4" r:id="rId4"/>
     <sheet name="Лист2" sheetId="5" r:id="rId5"/>
+    <sheet name="Лист3" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">th!$A$45:$C$507</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="63">
   <si>
     <t>T</t>
   </si>
@@ -205,6 +206,12 @@
   <si>
     <t>p2 exp / theory</t>
   </si>
+  <si>
+    <t>лет</t>
+  </si>
+  <si>
+    <t>дней всего</t>
+  </si>
 </sst>
 </file>
 
@@ -266,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,6 +293,7 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -29056,8 +29064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29481,4 +29489,137 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="15">
+        <v>40429</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="8">
+        <f ca="1">SUM(A1:A17)</f>
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <f>B2-B1</f>
+        <v>295</v>
+      </c>
+      <c r="B2" s="15">
+        <v>40724</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2">
+        <f ca="1">E1 /365</f>
+        <v>4.6630136986301371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="15">
+        <v>40787</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <f>B5-B4</f>
+        <v>303</v>
+      </c>
+      <c r="B5" s="15">
+        <v>41090</v>
+      </c>
+      <c r="D5">
+        <f>365-242</f>
+        <v>123</v>
+      </c>
+      <c r="E5">
+        <f>1702 - 365 * 4</f>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="15">
+        <v>41153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <f>B8-B7</f>
+        <v>302</v>
+      </c>
+      <c r="B8" s="15">
+        <v>41455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
+        <v>41541</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <f>B11-B10</f>
+        <v>279</v>
+      </c>
+      <c r="B11" s="15">
+        <v>41820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="15">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <f>B14-B13</f>
+        <v>40</v>
+      </c>
+      <c r="B14" s="15">
+        <v>41861</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="15">
+        <v>41884</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <f ca="1">B20-B16</f>
+        <v>483</v>
+      </c>
+      <c r="B17" s="15">
+        <v>41820</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
+        <f ca="1">TODAY()</f>
+        <v>42367</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>